<commit_message>
Updated the Valuation Files
</commit_message>
<xml_diff>
--- a/Opportunities/Park_PC_Valuation_v1.2.xlsx
+++ b/Opportunities/Park_PC_Valuation_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry.chen\PycharmProjects\pythonProject\Opportunities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC4846EA-5131-4CB4-B971-8711C7658FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E668EDC6-8E3B-4559-84DE-AADBCA8194CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{04C18DA2-D859-514B-9E1B-7E320FEEEDAF}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{04C18DA2-D859-514B-9E1B-7E320FEEEDAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="99">
   <si>
     <t>HKD</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Loan Amount:</t>
-  </si>
-  <si>
-    <t>Ideal Loan Amount</t>
   </si>
   <si>
     <t>Deal Analysis:</t>
@@ -556,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -678,17 +675,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="dotted">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -884,12 +870,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -918,7 +935,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -941,7 +957,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="169" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -978,16 +994,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="6" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -998,10 +1014,10 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,61 +1029,61 @@
     <xf numFmtId="6" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="7" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="8" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="8" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1079,8 +1095,8 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="8" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="8" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="38" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1096,14 +1112,15 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1139,25 +1156,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="16" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="16" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,53 +1192,53 @@
     <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="7" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="8" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="7" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="7" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="8" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="8" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="17" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1242,29 +1259,29 @@
     <xf numFmtId="170" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="6" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1594,7 +1611,7 @@
   <dimension ref="A2:I991"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1612,11 +1629,11 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="90" t="str">
+      <c r="C2" s="92" t="str">
         <f>C3&amp;" : "&amp;C4</f>
         <v>Park : Project Park</v>
       </c>
-      <c r="D2" s="91"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1625,37 +1642,37 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="92" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="93"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="94" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="95"/>
       <c r="E3" s="6"/>
       <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="94" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="95"/>
+      <c r="H3" s="96" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="97"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="97"/>
-      <c r="G4" s="55" t="s">
+      <c r="D4" s="99"/>
+      <c r="G4" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="60">
+      <c r="H4" s="59">
         <f>Securities!C5</f>
         <v>23880000</v>
       </c>
-      <c r="I4" s="61" t="str">
+      <c r="I4" s="60" t="str">
         <f>Securities!D4</f>
         <v>HKD</v>
       </c>
@@ -1664,30 +1681,30 @@
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="98">
+      <c r="C5" s="100">
         <v>44901</v>
       </c>
-      <c r="D5" s="97"/>
+      <c r="D5" s="99"/>
       <c r="E5" s="9"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="100">
+      <c r="C6" s="102">
         <v>44911</v>
       </c>
-      <c r="D6" s="101"/>
+      <c r="D6" s="103"/>
       <c r="E6" s="9" t="str">
         <f>IF(C6&lt;C5,"Outdated","")</f>
         <v/>
       </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1696,212 +1713,196 @@
       </c>
       <c r="C8" s="12"/>
       <c r="G8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="66">
+      <c r="D9" s="65">
         <v>5.3955400000000001E-2</v>
       </c>
       <c r="E9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="107">
+        <v>48</v>
+      </c>
+      <c r="H9" s="109">
         <f>Securities!C6</f>
         <v>0.62484472049689443</v>
       </c>
-      <c r="I9" s="107"/>
+      <c r="I9" s="109"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="85">
+      <c r="D10" s="84">
         <f>'Credit Analysis Model'!D52:E52</f>
         <v>2.8206030150753768E-3</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="30"/>
       <c r="G10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="106">
+        <v>38</v>
+      </c>
+      <c r="H10" s="108">
         <f>Securities!D7</f>
         <v>0.12</v>
       </c>
-      <c r="I10" s="106"/>
+      <c r="I10" s="108"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
-      <c r="E11" s="31"/>
+      <c r="E11" s="30"/>
       <c r="G11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="109">
+        <v>50</v>
+      </c>
+      <c r="H11" s="111">
         <f>Securities!C7</f>
         <v>2865600</v>
       </c>
-      <c r="I11" s="110"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="112"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="31"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="8"/>
-      <c r="G12" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="108">
+      <c r="G12" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="110">
         <f>Securities!C6</f>
         <v>0.62484472049689443</v>
       </c>
-      <c r="I12" s="108"/>
+      <c r="I12" s="110"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="31"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="17"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="31"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="17"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="105">
+      <c r="H14" s="31"/>
+      <c r="I14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="86"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="106"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="117"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="107">
         <f>H11</f>
         <v>2865600</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="G15" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="111">
+      <c r="D19" s="107"/>
+      <c r="G19" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="113">
         <f>H9</f>
         <v>0.62484472049689443</v>
       </c>
-      <c r="I15" s="111"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="87"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="104"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="13"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="115"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="I19" s="113"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="87"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="117">
-        <v>0</v>
-      </c>
-      <c r="D22" s="118"/>
-      <c r="E22" s="119" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="91"/>
+      <c r="G22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="119"/>
-      <c r="G22" s="120">
+      <c r="H22" s="122">
         <f>'Credit Analysis Model'!D55</f>
         <v>6.4027111830930822E-2</v>
       </c>
-      <c r="H22" s="120"/>
+      <c r="I22" s="123"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="121" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="121"/>
-      <c r="G23" s="122">
+      <c r="H23" s="124">
         <f>D9+D10</f>
         <v>5.6776003015075377E-2</v>
       </c>
-      <c r="H23" s="122"/>
+      <c r="I23" s="125"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="124" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="124"/>
-      <c r="G24" s="125">
-        <f>G22-G23</f>
+      <c r="B24" s="21"/>
+      <c r="C24" s="121"/>
+      <c r="D24" s="121"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="126">
+        <f>H22-H23</f>
         <v>7.2511088158554449E-3</v>
       </c>
-      <c r="H24" s="125"/>
-      <c r="I24" s="25"/>
+      <c r="I24" s="127"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="4"/>
@@ -1912,40 +1913,40 @@
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113"/>
-      <c r="G27" s="113"/>
-      <c r="H27" s="113"/>
-      <c r="I27" s="114"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="116"/>
     </row>
     <row r="28" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="127"/>
-      <c r="E28" s="127"/>
-      <c r="F28" s="127"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="127"/>
+      <c r="C28" s="128"/>
+      <c r="D28" s="129"/>
+      <c r="E28" s="129"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="128"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
     </row>
     <row r="29" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F30" s="18"/>
@@ -1953,73 +1954,73 @@
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="54"/>
+        <v>47</v>
+      </c>
+      <c r="C31" s="27"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="4"/>
       <c r="F31" s="10"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="129"/>
-      <c r="D32" s="130"/>
-      <c r="E32" s="129"/>
-      <c r="F32" s="130"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="131" t="s">
+      <c r="B32" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="131"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="131"/>
+      <c r="F32" s="132"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="131"/>
+      <c r="I32" s="133"/>
     </row>
     <row r="33" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="24"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="137"/>
-      <c r="E33" s="138"/>
-      <c r="F33" s="139"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="141"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="139"/>
+      <c r="E33" s="140"/>
+      <c r="F33" s="141"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="142"/>
+      <c r="I33" s="143"/>
     </row>
     <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="142">
-        <v>1</v>
-      </c>
-      <c r="D34" s="143"/>
-      <c r="E34" s="142">
-        <v>1</v>
-      </c>
-      <c r="F34" s="143"/>
-      <c r="G34" s="52">
-        <v>1</v>
-      </c>
-      <c r="H34" s="134">
+      <c r="B34" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="144">
+        <v>1</v>
+      </c>
+      <c r="D34" s="145"/>
+      <c r="E34" s="144">
+        <v>1</v>
+      </c>
+      <c r="F34" s="145"/>
+      <c r="G34" s="51">
+        <v>1</v>
+      </c>
+      <c r="H34" s="136">
         <f>C34+E34+G34</f>
         <v>3</v>
       </c>
-      <c r="I34" s="134"/>
+      <c r="I34" s="136"/>
     </row>
     <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="132"/>
-      <c r="D35" s="133"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="133"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="134">
+      <c r="B35" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="134"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="134"/>
+      <c r="F35" s="135"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="136">
         <f>C35+E35+G35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="135"/>
+      <c r="I35" s="137"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2978,7 +2979,7 @@
     <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="41">
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="H35:I35"/>
@@ -2999,25 +3000,21 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="H3:I3"/>
@@ -3025,7 +3022,7 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="H5:I5"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" sqref="H3" xr:uid="{A7845922-963A-9A4A-B0A0-331C191D0C34}">
       <formula1>"HK,US:NASDAQ,CN"</formula1>
     </dataValidation>
@@ -3060,372 +3057,372 @@
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="34"/>
+        <v>19</v>
+      </c>
+      <c r="C2" s="33"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="F3" s="46" t="s">
-        <v>41</v>
+      <c r="B3" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="F3" s="45" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="42">
+      <c r="B4" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="41">
         <f>SUM(C14+C22+C30)</f>
         <v>48300000</v>
       </c>
-      <c r="D4" s="146" t="str">
+      <c r="D4" s="148" t="str">
         <f>D14</f>
         <v>HKD</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="42">
+      <c r="B5" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="41">
         <f>SUM(,C16,C24,C32)</f>
         <v>23880000</v>
       </c>
-      <c r="D5" s="147"/>
-      <c r="F5" s="47" t="s">
-        <v>42</v>
+      <c r="D5" s="149"/>
+      <c r="F5" s="46" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="50">
+      <c r="B6" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="49">
         <f>(C5-C9)/C4</f>
         <v>0.62484472049689443</v>
       </c>
-      <c r="D6" s="51">
-        <v>1</v>
-      </c>
-      <c r="F6" s="47"/>
+      <c r="D6" s="50">
+        <v>1</v>
+      </c>
+      <c r="F6" s="46"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="45">
+      <c r="B7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="44">
         <f>C5*D7</f>
         <v>2865600</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="43">
         <v>0.12</v>
       </c>
-      <c r="F7" s="47"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="42">
+      <c r="B8" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="41">
         <f>SUM(C15,C23,C31)+C9</f>
         <v>22680000</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="61">
         <f>IF(C8/C5&gt;1,100%,C8/C5)</f>
         <v>0.94974874371859297</v>
       </c>
-      <c r="F8" s="47"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="43">
+      <c r="B9" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="42">
         <f>SUM(C18,C26,C34)</f>
         <v>-6300000</v>
       </c>
-      <c r="D9" s="62" t="str">
+      <c r="D9" s="61" t="str">
         <f>D17</f>
         <v>HKD</v>
       </c>
-      <c r="F9" s="47"/>
-    </row>
-    <row r="10" spans="1:6" s="38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="48"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:6" s="37" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="47"/>
+      <c r="B11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="148" t="s">
+      <c r="D12" s="150"/>
+      <c r="F12" s="46"/>
+    </row>
+    <row r="13" spans="1:6" ht="112" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="148"/>
-      <c r="F12" s="47"/>
-    </row>
-    <row r="13" spans="1:6" ht="112" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="36" t="s">
+      <c r="C13" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="148" t="s">
+      <c r="D13" s="150"/>
+      <c r="F13" s="46"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="148"/>
-      <c r="F13" s="47"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>18000000</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="47"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="45">
+      <c r="B15" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="44">
         <f>C14*D15</f>
         <v>10800000</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <v>0.6</v>
       </c>
-      <c r="F15" s="47" t="s">
-        <v>88</v>
+      <c r="F15" s="46" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="63">
+      <c r="B16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="62">
         <f>C14*D16+C18</f>
         <v>10800000</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <v>0.6</v>
       </c>
-      <c r="F16" s="47" t="s">
-        <v>43</v>
+      <c r="F16" s="46" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="43">
+      <c r="B17" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="42">
         <f>C14/8</f>
         <v>2250000</v>
       </c>
-      <c r="D17" s="144" t="s">
+      <c r="D17" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="47"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="43">
+      <c r="B18" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="42">
         <v>0</v>
       </c>
-      <c r="D18" s="145"/>
-      <c r="F18" s="49"/>
+      <c r="D18" s="147"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="47"/>
+      <c r="F19" s="46"/>
     </row>
     <row r="20" spans="2:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="150" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="150"/>
+      <c r="F20" s="46"/>
+    </row>
+    <row r="21" spans="2:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="150" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="148" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="148"/>
-      <c r="F20" s="47"/>
-    </row>
-    <row r="21" spans="2:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="148" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="148"/>
-      <c r="F21" s="47"/>
+      <c r="D21" s="150"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="2:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="42">
+      <c r="B22" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="41">
         <v>6300000</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="47"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="2:6" ht="14" x14ac:dyDescent="0.3">
-      <c r="B23" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="45">
+      <c r="B23" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="44">
         <f>C22*D23</f>
         <v>3780000</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="63">
         <v>0.6</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="63">
+      <c r="B24" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="62">
         <f>C22*D24+C26</f>
         <v>3780000</v>
       </c>
-      <c r="D24" s="64">
+      <c r="D24" s="63">
         <v>0.6</v>
       </c>
-      <c r="F24" s="47" t="s">
-        <v>44</v>
+      <c r="F24" s="46" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="43">
+      <c r="B25" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="42">
         <f>C22/545</f>
         <v>11559.633027522936</v>
       </c>
-      <c r="D25" s="144" t="s">
+      <c r="D25" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="47"/>
+      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="2:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="43">
+      <c r="B26" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="42">
         <v>0</v>
       </c>
-      <c r="D26" s="145"/>
-      <c r="F26" s="47"/>
+      <c r="D26" s="147"/>
+      <c r="F26" s="46"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="47"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="150"/>
+      <c r="F28" s="46"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="148" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="148"/>
-      <c r="F28" s="47"/>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="148" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="148"/>
-      <c r="F29" s="47"/>
+      <c r="D29" s="150"/>
+      <c r="F29" s="46"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="42">
+      <c r="B30" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="41">
         <v>24000000</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F30" s="47"/>
+      <c r="F30" s="46"/>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="45">
+      <c r="B31" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="44">
         <f>C30*D31</f>
         <v>14400000</v>
       </c>
-      <c r="D31" s="64">
+      <c r="D31" s="63">
         <v>0.6</v>
       </c>
-      <c r="F31" s="47" t="s">
-        <v>89</v>
+      <c r="F31" s="46" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="63">
+      <c r="B32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="62">
         <f>C30*D32+C34</f>
         <v>9300000</v>
       </c>
-      <c r="D32" s="64">
+      <c r="D32" s="63">
         <v>0.65</v>
       </c>
-      <c r="F32" s="47" t="s">
-        <v>45</v>
+      <c r="F32" s="46" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="43">
+      <c r="B33" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="42">
         <f>C30/1161</f>
         <v>20671.834625322997</v>
       </c>
-      <c r="D33" s="144" t="s">
+      <c r="D33" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="47"/>
+      <c r="F33" s="46"/>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="43">
+      <c r="B34" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="42">
         <v>-6300000</v>
       </c>
-      <c r="D34" s="145"/>
-      <c r="F34" s="47"/>
+      <c r="D34" s="147"/>
+      <c r="F34" s="46"/>
     </row>
     <row r="35" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="81"/>
+      <c r="C35" s="80"/>
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4407,11 +4404,11 @@
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="91"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="93"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -4421,69 +4418,69 @@
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="56">
+        <v>66</v>
+      </c>
+      <c r="D5" s="55">
         <f>Securities!C5</f>
         <v>23880000</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="68">
+        <v>56</v>
+      </c>
+      <c r="H5" s="67">
         <f>Securities!D8</f>
         <v>0.94974874371859297</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="68">
+        <v>34</v>
+      </c>
+      <c r="D6" s="67">
         <f>Securities!C6</f>
         <v>0.62484472049689443</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="68">
+        <v>67</v>
+      </c>
+      <c r="D7" s="67">
         <f>Securities!D7</f>
         <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="65"/>
+      <c r="B9" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="64"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="57" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="70">
+      <c r="B11" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="69">
         <f>-D5</f>
         <v>-23880000</v>
       </c>
-      <c r="E11" s="70">
+      <c r="E11" s="69">
         <f>D5*(1+D7)</f>
         <v>26745600.000000004</v>
       </c>
@@ -4493,1593 +4490,1593 @@
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="68">
         <f>IRR(D11:E11)</f>
         <v>0.12000000000000033</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.65" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="75">
+        <v>75</v>
+      </c>
+      <c r="D14" s="74">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="65"/>
+      <c r="B16" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="64"/>
     </row>
     <row r="17" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="71">
+      <c r="B17" s="37"/>
+      <c r="C17" s="70">
         <v>0</v>
       </c>
-      <c r="D17" s="71">
-        <v>1</v>
-      </c>
-      <c r="E17" s="71">
+      <c r="D17" s="70">
+        <v>1</v>
+      </c>
+      <c r="E17" s="70">
         <v>2</v>
       </c>
-      <c r="F17" s="71">
+      <c r="F17" s="70">
         <v>3</v>
       </c>
-      <c r="G17" s="71">
+      <c r="G17" s="70">
         <v>4</v>
       </c>
-      <c r="H17" s="71">
+      <c r="H17" s="70">
         <v>5</v>
       </c>
-      <c r="I17" s="71">
+      <c r="I17" s="70">
         <v>6</v>
       </c>
-      <c r="J17" s="71">
+      <c r="J17" s="70">
         <v>7</v>
       </c>
-      <c r="K17" s="71">
+      <c r="K17" s="70">
         <v>8</v>
       </c>
-      <c r="L17" s="71">
+      <c r="L17" s="70">
         <v>9</v>
       </c>
-      <c r="M17" s="71">
+      <c r="M17" s="70">
         <v>10</v>
       </c>
-      <c r="N17" s="71">
+      <c r="N17" s="70">
         <v>11</v>
       </c>
-      <c r="O17" s="71">
+      <c r="O17" s="70">
         <v>12</v>
       </c>
-      <c r="P17" s="77"/>
+      <c r="P17" s="76"/>
     </row>
     <row r="18" spans="2:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72">
+      <c r="B18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71">
         <f t="shared" ref="D18:O18" si="0">$D$7*100/12</f>
         <v>1</v>
       </c>
-      <c r="E18" s="72">
+      <c r="E18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H18" s="72">
+      <c r="H18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I18" s="72">
+      <c r="I18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J18" s="72">
+      <c r="J18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="72">
+      <c r="K18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L18" s="72">
+      <c r="L18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M18" s="72">
+      <c r="M18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N18" s="72">
+      <c r="N18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O18" s="72">
+      <c r="O18" s="71">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P18" s="82"/>
+      <c r="P18" s="81"/>
     </row>
     <row r="19" spans="2:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="72">
+      <c r="B19" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="71">
         <v>0</v>
       </c>
-      <c r="E19" s="72">
+      <c r="E19" s="71">
         <v>0</v>
       </c>
-      <c r="F19" s="72">
+      <c r="F19" s="71">
         <v>0</v>
       </c>
-      <c r="G19" s="72">
+      <c r="G19" s="71">
         <v>0</v>
       </c>
-      <c r="H19" s="72">
+      <c r="H19" s="71">
         <v>0</v>
       </c>
-      <c r="I19" s="72">
+      <c r="I19" s="71">
         <v>0</v>
       </c>
-      <c r="J19" s="72">
+      <c r="J19" s="71">
         <v>0</v>
       </c>
-      <c r="K19" s="72">
+      <c r="K19" s="71">
         <v>0</v>
       </c>
-      <c r="L19" s="72">
+      <c r="L19" s="71">
         <v>0</v>
       </c>
-      <c r="M19" s="72">
+      <c r="M19" s="71">
         <v>0</v>
       </c>
-      <c r="N19" s="72">
+      <c r="N19" s="71">
         <v>0</v>
       </c>
-      <c r="O19" s="72">
+      <c r="O19" s="71">
         <v>100</v>
       </c>
-      <c r="P19" s="82"/>
+      <c r="P19" s="81"/>
     </row>
     <row r="20" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="72">
+        <v>100</v>
+      </c>
+      <c r="E20" s="72">
+        <v>100</v>
+      </c>
+      <c r="F20" s="72">
+        <v>100</v>
+      </c>
+      <c r="G20" s="72">
+        <v>100</v>
+      </c>
+      <c r="H20" s="72">
+        <v>100</v>
+      </c>
+      <c r="I20" s="72">
+        <v>100</v>
+      </c>
+      <c r="J20" s="72">
+        <v>100</v>
+      </c>
+      <c r="K20" s="72">
+        <v>100</v>
+      </c>
+      <c r="L20" s="72">
+        <v>100</v>
+      </c>
+      <c r="M20" s="72">
+        <v>100</v>
+      </c>
+      <c r="N20" s="72">
+        <v>100</v>
+      </c>
+      <c r="O20" s="72">
+        <v>100</v>
+      </c>
+      <c r="P20" s="82"/>
+    </row>
+    <row r="21" spans="2:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="73">
-        <v>100</v>
-      </c>
-      <c r="E20" s="73">
-        <v>100</v>
-      </c>
-      <c r="F20" s="73">
-        <v>100</v>
-      </c>
-      <c r="G20" s="73">
-        <v>100</v>
-      </c>
-      <c r="H20" s="73">
-        <v>100</v>
-      </c>
-      <c r="I20" s="73">
-        <v>100</v>
-      </c>
-      <c r="J20" s="73">
-        <v>100</v>
-      </c>
-      <c r="K20" s="73">
-        <v>100</v>
-      </c>
-      <c r="L20" s="73">
-        <v>100</v>
-      </c>
-      <c r="M20" s="73">
-        <v>100</v>
-      </c>
-      <c r="N20" s="73">
-        <v>100</v>
-      </c>
-      <c r="O20" s="73">
-        <v>100</v>
-      </c>
-      <c r="P20" s="83"/>
-    </row>
-    <row r="21" spans="2:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="73">
+      <c r="C21" s="37"/>
+      <c r="D21" s="72">
         <f t="shared" ref="D21:O21" si="1">D20*$H$5</f>
         <v>94.9748743718593</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="G21" s="73">
+      <c r="G21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="I21" s="73">
+      <c r="I21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="J21" s="73">
+      <c r="J21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="K21" s="73">
+      <c r="K21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="L21" s="73">
+      <c r="L21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="M21" s="73">
+      <c r="M21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="N21" s="73">
+      <c r="N21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="O21" s="73">
+      <c r="O21" s="72">
         <f t="shared" si="1"/>
         <v>94.9748743718593</v>
       </c>
-      <c r="P21" s="83"/>
+      <c r="P21" s="82"/>
     </row>
     <row r="22" spans="2:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="74">
+      <c r="B22" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="73">
         <f t="shared" ref="D22:O22" si="2">D20-D21</f>
         <v>5.0251256281406995</v>
       </c>
-      <c r="E22" s="74">
+      <c r="E22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="G22" s="74">
+      <c r="G22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="H22" s="74">
+      <c r="H22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="J22" s="74">
+      <c r="J22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="K22" s="74">
+      <c r="K22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="L22" s="74">
+      <c r="L22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="M22" s="74">
+      <c r="M22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="N22" s="74">
+      <c r="N22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="O22" s="74">
+      <c r="O22" s="73">
         <f t="shared" si="2"/>
         <v>5.0251256281406995</v>
       </c>
-      <c r="P22" s="84"/>
+      <c r="P22" s="83"/>
     </row>
     <row r="23" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="68">
+      <c r="B23" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="67">
         <f>$D$50</f>
         <v>5.6129999999999999E-2</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="67">
         <f t="shared" ref="E23:O23" si="3">D24*$D$50</f>
         <v>5.2979423099999999E-2</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="67">
         <f t="shared" si="3"/>
         <v>5.0005688081397E-2</v>
       </c>
-      <c r="G23" s="68">
+      <c r="G23" s="67">
         <f t="shared" si="3"/>
         <v>4.7198868809388179E-2</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="67">
         <f t="shared" si="3"/>
         <v>4.4549596303117223E-2</v>
       </c>
-      <c r="I23" s="68">
+      <c r="I23" s="67">
         <f t="shared" si="3"/>
         <v>4.2049027462623255E-2</v>
       </c>
-      <c r="J23" s="68">
+      <c r="J23" s="67">
         <f t="shared" si="3"/>
         <v>3.9688815551146207E-2</v>
       </c>
-      <c r="K23" s="68">
+      <c r="K23" s="67">
         <f t="shared" si="3"/>
         <v>3.7461082334260376E-2</v>
       </c>
-      <c r="L23" s="68">
+      <c r="L23" s="67">
         <f t="shared" si="3"/>
         <v>3.5358391782838339E-2</v>
       </c>
-      <c r="M23" s="68">
+      <c r="M23" s="67">
         <f t="shared" si="3"/>
         <v>3.3373725252067617E-2</v>
       </c>
-      <c r="N23" s="68">
+      <c r="N23" s="67">
         <f t="shared" si="3"/>
         <v>3.1500458053669064E-2</v>
       </c>
-      <c r="O23" s="68">
+      <c r="O23" s="67">
         <f t="shared" si="3"/>
         <v>2.9732337343116619E-2</v>
       </c>
-      <c r="P23" s="85"/>
+      <c r="P23" s="84"/>
     </row>
     <row r="24" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="68">
+      <c r="B24" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="67">
         <f>1-D23</f>
         <v>0.94386999999999999</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="67">
         <f>D24-E23</f>
         <v>0.89089057689999995</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="67">
         <f t="shared" ref="F24:O24" si="4">E24-F23</f>
         <v>0.8408848888186029</v>
       </c>
-      <c r="G24" s="68">
+      <c r="G24" s="67">
         <f t="shared" si="4"/>
         <v>0.79368602000921473</v>
       </c>
-      <c r="H24" s="68">
+      <c r="H24" s="67">
         <f t="shared" si="4"/>
         <v>0.74913642370609757</v>
       </c>
-      <c r="I24" s="68">
+      <c r="I24" s="67">
         <f t="shared" si="4"/>
         <v>0.70708739624347428</v>
       </c>
-      <c r="J24" s="68">
+      <c r="J24" s="67">
         <f t="shared" si="4"/>
         <v>0.66739858069232805</v>
       </c>
-      <c r="K24" s="68">
+      <c r="K24" s="67">
         <f t="shared" si="4"/>
         <v>0.62993749835806767</v>
       </c>
-      <c r="L24" s="68">
+      <c r="L24" s="67">
         <f t="shared" si="4"/>
         <v>0.59457910657522928</v>
       </c>
-      <c r="M24" s="68">
+      <c r="M24" s="67">
         <f t="shared" si="4"/>
         <v>0.56120538132316167</v>
       </c>
-      <c r="N24" s="68">
+      <c r="N24" s="67">
         <f t="shared" si="4"/>
         <v>0.52970492326949259</v>
       </c>
-      <c r="O24" s="68">
+      <c r="O24" s="67">
         <f t="shared" si="4"/>
         <v>0.49997258592637595</v>
       </c>
-      <c r="P24" s="85"/>
-      <c r="Q24" s="25"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="24"/>
     </row>
     <row r="25" spans="2:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="72">
+      <c r="B25" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="71">
         <f>D22*D23</f>
         <v>0.28206030150753747</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="71">
         <f t="shared" ref="E25:O25" si="5">E22*E23</f>
         <v>0.26622825678391937</v>
       </c>
-      <c r="F25" s="72">
+      <c r="F25" s="71">
         <f t="shared" si="5"/>
         <v>0.25128486473063799</v>
       </c>
-      <c r="G25" s="72">
+      <c r="G25" s="71">
         <f t="shared" si="5"/>
         <v>0.23718024527330725</v>
       </c>
-      <c r="H25" s="72">
+      <c r="H25" s="71">
         <f t="shared" si="5"/>
         <v>0.22386731810611651</v>
       </c>
-      <c r="I25" s="72">
+      <c r="I25" s="71">
         <f t="shared" si="5"/>
         <v>0.2113016455408202</v>
       </c>
-      <c r="J25" s="72">
+      <c r="J25" s="71">
         <f t="shared" si="5"/>
         <v>0.19944128417661394</v>
       </c>
-      <c r="K25" s="72">
+      <c r="K25" s="71">
         <f t="shared" si="5"/>
         <v>0.18824664489578063</v>
       </c>
-      <c r="L25" s="72">
+      <c r="L25" s="71">
         <f t="shared" si="5"/>
         <v>0.17768036071778046</v>
       </c>
-      <c r="M25" s="72">
+      <c r="M25" s="71">
         <f t="shared" si="5"/>
         <v>0.16770716207069142</v>
       </c>
-      <c r="N25" s="72">
+      <c r="N25" s="71">
         <f t="shared" si="5"/>
         <v>0.15829375906366352</v>
       </c>
-      <c r="O25" s="72">
+      <c r="O25" s="71">
         <f t="shared" si="5"/>
         <v>0.14940873036742008</v>
       </c>
-      <c r="P25" s="82"/>
+      <c r="P25" s="81"/>
     </row>
     <row r="26" spans="2:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="68">
+      <c r="B26" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^D17)</f>
         <v>0.99552384273796135</v>
       </c>
-      <c r="E26" s="68">
+      <c r="E26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^E17)</f>
         <v>0.99106772145975719</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^F17)</f>
         <v>0.98663154648117291</v>
       </c>
-      <c r="G26" s="68">
+      <c r="G26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^G17)</f>
         <v>0.98221522851943488</v>
       </c>
-      <c r="H26" s="68">
+      <c r="H26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^H17)</f>
         <v>0.9778186786914127</v>
       </c>
-      <c r="I26" s="68">
+      <c r="I26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^I17)</f>
         <v>0.97344180851183104</v>
       </c>
-      <c r="J26" s="68">
+      <c r="J26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^J17)</f>
         <v>0.96908452989148874</v>
       </c>
-      <c r="K26" s="68">
+      <c r="K26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^K17)</f>
         <v>0.9647467551354858</v>
       </c>
-      <c r="L26" s="68">
+      <c r="L26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^L17)</f>
         <v>0.96042839694145798</v>
       </c>
-      <c r="M26" s="68">
+      <c r="M26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^M17)</f>
         <v>0.95612936839782037</v>
       </c>
-      <c r="N26" s="68">
+      <c r="N26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^N17)</f>
         <v>0.95184958298201783</v>
       </c>
-      <c r="O26" s="68">
+      <c r="O26" s="67">
         <f>1/((1+Dashboard!$D$9/12)^O17)</f>
         <v>0.94758895455878456</v>
       </c>
-      <c r="P26" s="85"/>
-      <c r="Q26" s="76" t="s">
-        <v>77</v>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="75" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:17" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="72">
+      <c r="B27" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="37"/>
+      <c r="D27" s="71">
         <f>D25*D26</f>
         <v>0.28079775524061168</v>
       </c>
-      <c r="E27" s="72">
+      <c r="E27" s="71">
         <f t="shared" ref="E27:O27" si="6">E25*E26</f>
         <v>0.2638502318390421</v>
       </c>
-      <c r="F27" s="72">
+      <c r="F27" s="71">
         <f t="shared" si="6"/>
         <v>0.2479255746965017</v>
       </c>
-      <c r="G27" s="72">
+      <c r="G27" s="71">
         <f t="shared" si="6"/>
         <v>0.23296204881141711</v>
       </c>
-      <c r="H27" s="72">
+      <c r="H27" s="71">
         <f t="shared" si="6"/>
         <v>0.21890164519271302</v>
       </c>
-      <c r="I27" s="72">
+      <c r="I27" s="71">
         <f t="shared" si="6"/>
         <v>0.20568985597678191</v>
       </c>
-      <c r="J27" s="72">
+      <c r="J27" s="71">
         <f t="shared" si="6"/>
         <v>0.19327546311724875</v>
       </c>
-      <c r="K27" s="72">
+      <c r="K27" s="71">
         <f t="shared" si="6"/>
         <v>0.18161033982834643</v>
       </c>
-      <c r="L27" s="72">
+      <c r="L27" s="71">
         <f t="shared" si="6"/>
         <v>0.17064926401215788</v>
       </c>
-      <c r="M27" s="72">
+      <c r="M27" s="71">
         <f t="shared" si="6"/>
         <v>0.16034974294644108</v>
       </c>
-      <c r="N27" s="72">
+      <c r="N27" s="71">
         <f t="shared" si="6"/>
         <v>0.15067184855340413</v>
       </c>
-      <c r="O27" s="72">
+      <c r="O27" s="71">
         <f t="shared" si="6"/>
         <v>0.14157806261081893</v>
       </c>
-      <c r="P27" s="72"/>
-      <c r="Q27" s="72">
+      <c r="P27" s="71"/>
+      <c r="Q27" s="71">
         <f>SUM(D27:O27)</f>
         <v>2.4482618328254842</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="65"/>
+      <c r="B29" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="64"/>
     </row>
     <row r="30" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="70">
+        <v>0</v>
+      </c>
+      <c r="D30" s="70">
+        <v>1</v>
+      </c>
+      <c r="E30" s="70">
+        <v>2</v>
+      </c>
+      <c r="F30" s="70">
+        <v>3</v>
+      </c>
+      <c r="G30" s="70">
+        <v>4</v>
+      </c>
+      <c r="H30" s="70">
+        <v>5</v>
+      </c>
+      <c r="I30" s="70">
+        <v>6</v>
+      </c>
+      <c r="J30" s="70">
+        <v>7</v>
+      </c>
+      <c r="K30" s="70">
+        <v>8</v>
+      </c>
+      <c r="L30" s="70">
+        <v>9</v>
+      </c>
+      <c r="M30" s="70">
+        <v>10</v>
+      </c>
+      <c r="N30" s="70">
+        <v>11</v>
+      </c>
+      <c r="O30" s="70">
+        <v>12</v>
+      </c>
+      <c r="P30" s="76"/>
+      <c r="Q30" s="32"/>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="71">
-        <v>0</v>
-      </c>
-      <c r="D30" s="71">
-        <v>1</v>
-      </c>
-      <c r="E30" s="71">
-        <v>2</v>
-      </c>
-      <c r="F30" s="71">
-        <v>3</v>
-      </c>
-      <c r="G30" s="71">
-        <v>4</v>
-      </c>
-      <c r="H30" s="71">
-        <v>5</v>
-      </c>
-      <c r="I30" s="71">
-        <v>6</v>
-      </c>
-      <c r="J30" s="71">
-        <v>7</v>
-      </c>
-      <c r="K30" s="71">
-        <v>8</v>
-      </c>
-      <c r="L30" s="71">
-        <v>9</v>
-      </c>
-      <c r="M30" s="71">
-        <v>10</v>
-      </c>
-      <c r="N30" s="71">
-        <v>11</v>
-      </c>
-      <c r="O30" s="71">
-        <v>12</v>
-      </c>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="33"/>
-    </row>
-    <row r="31" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="78">
+      <c r="C31" s="77">
         <f t="shared" ref="C31:C43" si="7">-$D$14+$C$18</f>
         <v>-100</v>
       </c>
-      <c r="D31" s="78">
+      <c r="D31" s="77">
         <f>D21+D18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="78"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
     </row>
     <row r="32" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="71">
+      <c r="B32" s="70">
         <v>2</v>
       </c>
-      <c r="C32" s="78">
+      <c r="C32" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D32" s="78">
+      <c r="D32" s="77">
         <f t="shared" ref="D32:D43" si="8">$D$18</f>
         <v>1</v>
       </c>
-      <c r="E32" s="78">
+      <c r="E32" s="77">
         <f>E21+E18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="78"/>
-      <c r="P32" s="78"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
     </row>
     <row r="33" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="71">
+      <c r="B33" s="70">
         <v>3</v>
       </c>
-      <c r="C33" s="78">
+      <c r="C33" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D33" s="78">
+      <c r="D33" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E33" s="78">
+      <c r="E33" s="77">
         <f t="shared" ref="E33:E43" si="9">$E$18</f>
         <v>1</v>
       </c>
-      <c r="F33" s="78">
+      <c r="F33" s="77">
         <f>F21+F18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="78"/>
-      <c r="L33" s="78"/>
-      <c r="M33" s="78"/>
-      <c r="N33" s="78"/>
-      <c r="O33" s="78"/>
-      <c r="P33" s="78"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
     </row>
     <row r="34" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="71">
+      <c r="B34" s="70">
         <v>4</v>
       </c>
-      <c r="C34" s="78">
+      <c r="C34" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D34" s="78">
+      <c r="D34" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E34" s="78">
+      <c r="E34" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F34" s="78">
+      <c r="F34" s="77">
         <f t="shared" ref="F34:F43" si="10">$F$18</f>
         <v>1</v>
       </c>
-      <c r="G34" s="78">
+      <c r="G34" s="77">
         <f>G21+G18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="78"/>
-      <c r="N34" s="78"/>
-      <c r="O34" s="78"/>
-      <c r="P34" s="78"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
     </row>
     <row r="35" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="71">
+      <c r="B35" s="70">
         <v>5</v>
       </c>
-      <c r="C35" s="78">
+      <c r="C35" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D35" s="78">
+      <c r="D35" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E35" s="78">
+      <c r="E35" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F35" s="78">
+      <c r="F35" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G35" s="78">
+      <c r="G35" s="77">
         <f t="shared" ref="G35:G43" si="11">$F$18</f>
         <v>1</v>
       </c>
-      <c r="H35" s="78">
+      <c r="H35" s="77">
         <f>H21+H18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
-      <c r="L35" s="78"/>
-      <c r="M35" s="78"/>
-      <c r="N35" s="78"/>
-      <c r="O35" s="78"/>
-      <c r="P35" s="78"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="77"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
     </row>
     <row r="36" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="71">
+      <c r="B36" s="70">
         <v>6</v>
       </c>
-      <c r="C36" s="78">
+      <c r="C36" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D36" s="78">
+      <c r="D36" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E36" s="78">
+      <c r="E36" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F36" s="78">
+      <c r="F36" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G36" s="78">
+      <c r="G36" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H36" s="78">
+      <c r="H36" s="77">
         <f t="shared" ref="H36:H43" si="12">$F$18</f>
         <v>1</v>
       </c>
-      <c r="I36" s="78">
+      <c r="I36" s="77">
         <f>I21+I18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
-      <c r="M36" s="78"/>
-      <c r="N36" s="78"/>
-      <c r="O36" s="78"/>
-      <c r="P36" s="78"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="77"/>
+      <c r="L36" s="77"/>
+      <c r="M36" s="77"/>
+      <c r="N36" s="77"/>
+      <c r="O36" s="77"/>
+      <c r="P36" s="77"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="71">
+      <c r="B37" s="70">
         <v>7</v>
       </c>
-      <c r="C37" s="78">
+      <c r="C37" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D37" s="78">
+      <c r="D37" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E37" s="78">
+      <c r="E37" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F37" s="78">
+      <c r="F37" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G37" s="78">
+      <c r="G37" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H37" s="78">
+      <c r="H37" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I37" s="78">
+      <c r="I37" s="77">
         <f t="shared" ref="I37:I43" si="13">$F$18</f>
         <v>1</v>
       </c>
-      <c r="J37" s="78">
+      <c r="J37" s="77">
         <f>J21+J18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="K37" s="78"/>
-      <c r="L37" s="78"/>
-      <c r="M37" s="78"/>
-      <c r="N37" s="78"/>
-      <c r="O37" s="78"/>
-      <c r="P37" s="78"/>
+      <c r="K37" s="77"/>
+      <c r="L37" s="77"/>
+      <c r="M37" s="77"/>
+      <c r="N37" s="77"/>
+      <c r="O37" s="77"/>
+      <c r="P37" s="77"/>
     </row>
     <row r="38" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="71">
+      <c r="B38" s="70">
         <v>8</v>
       </c>
-      <c r="C38" s="78">
+      <c r="C38" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D38" s="78">
+      <c r="D38" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E38" s="78">
+      <c r="E38" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F38" s="78">
+      <c r="F38" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G38" s="78">
+      <c r="G38" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H38" s="78">
+      <c r="H38" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I38" s="78">
+      <c r="I38" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J38" s="78">
+      <c r="J38" s="77">
         <f t="shared" ref="J38:J43" si="14">$F$18</f>
         <v>1</v>
       </c>
-      <c r="K38" s="78">
+      <c r="K38" s="77">
         <f>K21+K18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="L38" s="78"/>
-      <c r="M38" s="78"/>
-      <c r="N38" s="78"/>
-      <c r="O38" s="78"/>
-      <c r="P38" s="78"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="77"/>
+      <c r="O38" s="77"/>
+      <c r="P38" s="77"/>
     </row>
     <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="71">
+      <c r="B39" s="70">
         <v>9</v>
       </c>
-      <c r="C39" s="78">
+      <c r="C39" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D39" s="78">
+      <c r="D39" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E39" s="78">
+      <c r="E39" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F39" s="78">
+      <c r="F39" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G39" s="78">
+      <c r="G39" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H39" s="78">
+      <c r="H39" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I39" s="78">
+      <c r="I39" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J39" s="78">
+      <c r="J39" s="77">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K39" s="78">
+      <c r="K39" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="L39" s="78">
+      <c r="L39" s="77">
         <f>L21+L18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="M39" s="78"/>
-      <c r="N39" s="78"/>
-      <c r="O39" s="78"/>
-      <c r="P39" s="78"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="77"/>
+      <c r="P39" s="77"/>
     </row>
     <row r="40" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="71">
+      <c r="B40" s="70">
         <v>10</v>
       </c>
-      <c r="C40" s="78">
+      <c r="C40" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D40" s="78">
+      <c r="D40" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E40" s="78">
+      <c r="E40" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F40" s="78">
+      <c r="F40" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G40" s="78">
+      <c r="G40" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H40" s="78">
+      <c r="H40" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I40" s="78">
+      <c r="I40" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J40" s="78">
+      <c r="J40" s="77">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K40" s="78">
+      <c r="K40" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="L40" s="78">
+      <c r="L40" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="M40" s="78">
+      <c r="M40" s="77">
         <f>M21+M18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="N40" s="78"/>
-      <c r="O40" s="78"/>
-      <c r="P40" s="78"/>
+      <c r="N40" s="77"/>
+      <c r="O40" s="77"/>
+      <c r="P40" s="77"/>
     </row>
     <row r="41" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="71">
+      <c r="B41" s="70">
         <v>11</v>
       </c>
-      <c r="C41" s="78">
+      <c r="C41" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D41" s="78">
+      <c r="D41" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E41" s="78">
+      <c r="E41" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F41" s="78">
+      <c r="F41" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G41" s="78">
+      <c r="G41" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H41" s="78">
+      <c r="H41" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I41" s="78">
+      <c r="I41" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J41" s="78">
+      <c r="J41" s="77">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K41" s="78">
+      <c r="K41" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="L41" s="78">
+      <c r="L41" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="M41" s="78">
+      <c r="M41" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="N41" s="78">
+      <c r="N41" s="77">
         <f>N21+N18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="O41" s="78"/>
-      <c r="P41" s="78"/>
+      <c r="O41" s="77"/>
+      <c r="P41" s="77"/>
     </row>
     <row r="42" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="71">
+      <c r="B42" s="70">
         <v>12</v>
       </c>
-      <c r="C42" s="78">
+      <c r="C42" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D42" s="78">
+      <c r="D42" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E42" s="78">
+      <c r="E42" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F42" s="78">
+      <c r="F42" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G42" s="78">
+      <c r="G42" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H42" s="78">
+      <c r="H42" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I42" s="78">
+      <c r="I42" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J42" s="78">
+      <c r="J42" s="77">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K42" s="78">
+      <c r="K42" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="L42" s="78">
+      <c r="L42" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="M42" s="78">
+      <c r="M42" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="N42" s="78">
+      <c r="N42" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="O42" s="78">
+      <c r="O42" s="77">
         <f>O21+O18</f>
         <v>95.9748743718593</v>
       </c>
-      <c r="P42" s="78"/>
+      <c r="P42" s="77"/>
     </row>
     <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="78">
+      <c r="B43" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="77">
         <f t="shared" si="7"/>
         <v>-100</v>
       </c>
-      <c r="D43" s="78">
+      <c r="D43" s="77">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E43" s="78">
+      <c r="E43" s="77">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F43" s="78">
+      <c r="F43" s="77">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G43" s="78">
+      <c r="G43" s="77">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H43" s="78">
+      <c r="H43" s="77">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="I43" s="78">
+      <c r="I43" s="77">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="J43" s="78">
+      <c r="J43" s="77">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="K43" s="78">
+      <c r="K43" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="L43" s="78">
+      <c r="L43" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="M43" s="78">
+      <c r="M43" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="N43" s="78">
+      <c r="N43" s="77">
         <f>$F$18</f>
         <v>1</v>
       </c>
-      <c r="O43" s="78">
+      <c r="O43" s="77">
         <f>100+O18</f>
         <v>101</v>
       </c>
-      <c r="P43" s="78"/>
+      <c r="P43" s="77"/>
     </row>
     <row r="44" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
     </row>
     <row r="45" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="79"/>
-      <c r="D45" s="71">
-        <v>1</v>
-      </c>
-      <c r="E45" s="71">
+      <c r="B45" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="78"/>
+      <c r="D45" s="70">
+        <v>1</v>
+      </c>
+      <c r="E45" s="70">
         <v>2</v>
       </c>
-      <c r="F45" s="71">
+      <c r="F45" s="70">
         <v>3</v>
       </c>
-      <c r="G45" s="71">
+      <c r="G45" s="70">
         <v>4</v>
       </c>
-      <c r="H45" s="71">
+      <c r="H45" s="70">
         <v>5</v>
       </c>
-      <c r="I45" s="71">
+      <c r="I45" s="70">
         <v>6</v>
       </c>
-      <c r="J45" s="71">
+      <c r="J45" s="70">
         <v>7</v>
       </c>
-      <c r="K45" s="71">
+      <c r="K45" s="70">
         <v>8</v>
       </c>
-      <c r="L45" s="71">
+      <c r="L45" s="70">
         <v>9</v>
       </c>
-      <c r="M45" s="71">
+      <c r="M45" s="70">
         <v>10</v>
       </c>
-      <c r="N45" s="71">
+      <c r="N45" s="70">
         <v>11</v>
       </c>
-      <c r="O45" s="71">
+      <c r="O45" s="70">
         <v>12</v>
       </c>
-      <c r="Q45" s="57" t="s">
-        <v>91</v>
+      <c r="Q45" s="56" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="2:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="79"/>
-      <c r="D46" s="68">
+      <c r="B46" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="78"/>
+      <c r="D46" s="67">
         <f>C31/D31+1</f>
         <v>-4.1939368553327361E-2</v>
       </c>
-      <c r="E46" s="68">
+      <c r="E46" s="67">
         <f>IRR($C$32:E32)</f>
         <v>-1.531957061570699E-2</v>
       </c>
-      <c r="F46" s="68">
+      <c r="F46" s="67">
         <f>IRR($C$33:F33)</f>
         <v>-6.8659546112914693E-3</v>
       </c>
-      <c r="G46" s="68">
+      <c r="G46" s="67">
         <f>IRR($C34:G$34)</f>
         <v>-2.6121452019300939E-3</v>
       </c>
-      <c r="H46" s="68">
+      <c r="H46" s="67">
         <f>IRR($C$35:H35)</f>
         <v>-5.1282105228200869E-5</v>
       </c>
-      <c r="I46" s="68">
+      <c r="I46" s="67">
         <f>IRR($C$36:I36)</f>
         <v>1.6594694152978207E-3</v>
       </c>
-      <c r="J46" s="68">
+      <c r="J46" s="67">
         <f>IRR($C$37:J37)</f>
         <v>2.8831019754969045E-3</v>
       </c>
-      <c r="K46" s="68">
+      <c r="K46" s="67">
         <f>IRR($C$38:K38)</f>
         <v>3.8016972852410458E-3</v>
       </c>
-      <c r="L46" s="68">
+      <c r="L46" s="67">
         <f>IRR($C$39:L39)</f>
         <v>4.5166436865142767E-3</v>
       </c>
-      <c r="M46" s="68">
+      <c r="M46" s="67">
         <f>IRR($C$40:M40)</f>
         <v>5.0888786803384711E-3</v>
       </c>
-      <c r="N46" s="68">
+      <c r="N46" s="67">
         <f>IRR($C$41:N41)</f>
         <v>5.5572325605750539E-3</v>
       </c>
-      <c r="O46" s="68">
+      <c r="O46" s="67">
         <f>IRR($C$42:O42)</f>
         <v>5.9476199828485399E-3</v>
       </c>
-      <c r="Q46" s="68">
+      <c r="Q46" s="67">
         <f>IRR($C$43:O43)</f>
         <v>1.0000000000000231E-2</v>
       </c>
     </row>
     <row r="47" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="77"/>
-      <c r="D47" s="50">
+      <c r="B47" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="76"/>
+      <c r="D47" s="49">
         <f>D46*D45</f>
         <v>-4.1939368553327361E-2</v>
       </c>
-      <c r="E47" s="50">
+      <c r="E47" s="49">
         <f t="shared" ref="E47:O47" si="15">E46*E45</f>
         <v>-3.063914123141398E-2</v>
       </c>
-      <c r="F47" s="50">
+      <c r="F47" s="49">
         <f t="shared" si="15"/>
         <v>-2.0597863833874408E-2</v>
       </c>
-      <c r="G47" s="50">
+      <c r="G47" s="49">
         <f t="shared" si="15"/>
         <v>-1.0448580807720376E-2</v>
       </c>
-      <c r="H47" s="50">
+      <c r="H47" s="49">
         <f t="shared" si="15"/>
         <v>-2.5641052614100435E-4</v>
       </c>
-      <c r="I47" s="50">
+      <c r="I47" s="49">
         <f t="shared" si="15"/>
         <v>9.956816491786924E-3</v>
       </c>
-      <c r="J47" s="50">
+      <c r="J47" s="49">
         <f t="shared" si="15"/>
         <v>2.0181713828478332E-2</v>
       </c>
-      <c r="K47" s="50">
+      <c r="K47" s="49">
         <f t="shared" si="15"/>
         <v>3.0413578281928366E-2</v>
       </c>
-      <c r="L47" s="50">
+      <c r="L47" s="49">
         <f t="shared" si="15"/>
         <v>4.0649793178628491E-2</v>
       </c>
-      <c r="M47" s="50">
+      <c r="M47" s="49">
         <f t="shared" si="15"/>
         <v>5.0888786803384711E-2</v>
       </c>
-      <c r="N47" s="50">
+      <c r="N47" s="49">
         <f t="shared" si="15"/>
         <v>6.1129558166325593E-2</v>
       </c>
-      <c r="O47" s="50">
+      <c r="O47" s="49">
         <f t="shared" si="15"/>
         <v>7.1371439794182479E-2</v>
       </c>
-      <c r="Q47" s="68">
+      <c r="Q47" s="67">
         <f t="shared" ref="Q47" si="16">Q46*12</f>
         <v>0.12000000000000277</v>
       </c>
     </row>
     <row r="48" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="65" t="s">
-        <v>16</v>
+      <c r="B49" s="64" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="69">
+        <v>58</v>
+      </c>
+      <c r="D50" s="68">
         <v>5.6129999999999999E-2</v>
       </c>
-      <c r="E50" s="86" t="s">
-        <v>75</v>
+      <c r="E50" s="85" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C51" s="77"/>
-      <c r="D51" s="149">
+        <v>93</v>
+      </c>
+      <c r="C51" s="76"/>
+      <c r="D51" s="151">
         <f>SUM(D23:O23)</f>
         <v>0.50002741407362383</v>
       </c>
-      <c r="E51" s="149"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="77"/>
-      <c r="J51" s="77"/>
-      <c r="K51" s="77"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
-      <c r="N51" s="78"/>
-      <c r="O51" s="78"/>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="78"/>
+      <c r="E51" s="151"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="77"/>
+      <c r="O51" s="77"/>
+      <c r="P51" s="84"/>
+      <c r="Q51" s="77"/>
     </row>
     <row r="52" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="150">
+        <v>57</v>
+      </c>
+      <c r="D52" s="152">
         <f>(1-H5)*D50</f>
         <v>2.8206030150753768E-3</v>
       </c>
-      <c r="E52" s="150"/>
+      <c r="E52" s="152"/>
     </row>
     <row r="53" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" s="77"/>
-      <c r="D54" s="68">
+      <c r="B54" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="76"/>
+      <c r="D54" s="67">
         <f t="shared" ref="D54:O54" si="17">D23*D47</f>
         <v>-2.3540567568982648E-3</v>
       </c>
-      <c r="E54" s="68">
+      <c r="E54" s="67">
         <f t="shared" si="17"/>
         <v>-1.6232440267197363E-3</v>
       </c>
-      <c r="F54" s="68">
+      <c r="F54" s="67">
         <f t="shared" si="17"/>
         <v>-1.0300103540198118E-3</v>
       </c>
-      <c r="G54" s="68">
+      <c r="G54" s="67">
         <f t="shared" si="17"/>
         <v>-4.9316119478788514E-4</v>
       </c>
-      <c r="H54" s="68">
+      <c r="H54" s="67">
         <f t="shared" si="17"/>
         <v>-1.1422985427451629E-5</v>
       </c>
-      <c r="I54" s="68">
+      <c r="I54" s="67">
         <f t="shared" si="17"/>
         <v>4.186744501034485E-4</v>
       </c>
-      <c r="J54" s="68">
+      <c r="J54" s="67">
         <f t="shared" si="17"/>
         <v>8.0098831764449326E-4</v>
       </c>
-      <c r="K54" s="68">
+      <c r="K54" s="67">
         <f t="shared" si="17"/>
         <v>1.1393255600987918E-3</v>
       </c>
-      <c r="L54" s="68">
+      <c r="L54" s="67">
         <f t="shared" si="17"/>
         <v>1.4373113131012955E-3</v>
       </c>
-      <c r="M54" s="68">
+      <c r="M54" s="67">
         <f t="shared" si="17"/>
         <v>1.6983483891872056E-3</v>
       </c>
-      <c r="N54" s="68">
+      <c r="N54" s="67">
         <f t="shared" si="17"/>
         <v>1.9256090828576626E-3</v>
       </c>
-      <c r="O54" s="68">
+      <c r="O54" s="67">
         <f t="shared" si="17"/>
         <v>2.1220397246245713E-3</v>
       </c>
-      <c r="Q54" s="68">
+      <c r="Q54" s="67">
         <f>O24*Q47</f>
         <v>5.9996710311166497E-2</v>
       </c>
     </row>
     <row r="55" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="77"/>
-      <c r="D55" s="80">
+      <c r="B55" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="76"/>
+      <c r="D55" s="79">
         <f>SUM(D54:Q54)</f>
         <v>6.4027111830930822E-2</v>
       </c>
-      <c r="E55" s="77"/>
-      <c r="F55" s="77"/>
-      <c r="G55" s="77"/>
-      <c r="H55" s="77"/>
-      <c r="I55" s="77"/>
-      <c r="J55" s="77"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="77"/>
-      <c r="N55" s="78"/>
-      <c r="O55" s="78"/>
-      <c r="P55" s="77"/>
-      <c r="Q55" s="78"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="77"/>
+      <c r="O55" s="77"/>
+      <c r="P55" s="76"/>
+      <c r="Q55" s="77"/>
     </row>
     <row r="56" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="33"/>
-      <c r="C56" s="77"/>
-      <c r="D56" s="77"/>
-      <c r="E56" s="77"/>
-      <c r="F56" s="77"/>
-      <c r="G56" s="77"/>
-      <c r="H56" s="77"/>
-      <c r="I56" s="77"/>
-      <c r="J56" s="77"/>
-      <c r="K56" s="77"/>
-      <c r="L56" s="77"/>
-      <c r="M56" s="77"/>
-      <c r="N56" s="78"/>
-      <c r="O56" s="78"/>
-      <c r="P56" s="78"/>
-      <c r="Q56" s="78"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="77"/>
+      <c r="O56" s="77"/>
+      <c r="P56" s="77"/>
+      <c r="Q56" s="77"/>
     </row>
     <row r="57" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="33"/>
-      <c r="C57" s="77"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="77"/>
-      <c r="F57" s="77"/>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="77"/>
-      <c r="N57" s="78"/>
-      <c r="O57" s="78"/>
-      <c r="P57" s="78"/>
-      <c r="Q57" s="78"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="77"/>
+      <c r="O57" s="77"/>
+      <c r="P57" s="77"/>
+      <c r="Q57" s="77"/>
     </row>
     <row r="58" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="33"/>
-      <c r="C58" s="77"/>
-      <c r="D58" s="77"/>
-      <c r="E58" s="77"/>
-      <c r="F58" s="77"/>
-      <c r="G58" s="77"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="77"/>
-      <c r="J58" s="77"/>
-      <c r="K58" s="77"/>
-      <c r="L58" s="77"/>
-      <c r="M58" s="77"/>
-      <c r="N58" s="78"/>
-      <c r="O58" s="78"/>
-      <c r="P58" s="78"/>
-      <c r="Q58" s="78"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="76"/>
+      <c r="I58" s="76"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="76"/>
+      <c r="M58" s="76"/>
+      <c r="N58" s="77"/>
+      <c r="O58" s="77"/>
+      <c r="P58" s="77"/>
+      <c r="Q58" s="77"/>
     </row>
     <row r="59" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="33"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="77"/>
-      <c r="F59" s="77"/>
-      <c r="G59" s="77"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="77"/>
-      <c r="J59" s="77"/>
-      <c r="K59" s="77"/>
-      <c r="L59" s="77"/>
-      <c r="M59" s="77"/>
-      <c r="N59" s="78"/>
-      <c r="O59" s="78"/>
-      <c r="P59" s="78"/>
-      <c r="Q59" s="78"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="76"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="77"/>
+      <c r="O59" s="77"/>
+      <c r="P59" s="77"/>
+      <c r="Q59" s="77"/>
     </row>
     <row r="60" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E60" s="78"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="78"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="78"/>
-      <c r="J60" s="78"/>
-      <c r="K60" s="78"/>
-      <c r="L60" s="78"/>
-      <c r="M60" s="78"/>
-      <c r="N60" s="78"/>
-      <c r="O60" s="78"/>
-      <c r="P60" s="78"/>
-      <c r="Q60" s="78"/>
+      <c r="E60" s="77"/>
+      <c r="F60" s="77"/>
+      <c r="G60" s="77"/>
+      <c r="H60" s="77"/>
+      <c r="I60" s="77"/>
+      <c r="J60" s="77"/>
+      <c r="K60" s="77"/>
+      <c r="L60" s="77"/>
+      <c r="M60" s="77"/>
+      <c r="N60" s="77"/>
+      <c r="O60" s="77"/>
+      <c r="P60" s="77"/>
+      <c r="Q60" s="77"/>
     </row>
     <row r="61" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>